<commit_message>
Added motor control section
</commit_message>
<xml_diff>
--- a/docs/pi_hat_docs/GPIO_Pinout.xlsx
+++ b/docs/pi_hat_docs/GPIO_Pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Graeme\Desktop\solar_tracking_project\Hardware\pi_hat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A409C88-612F-4562-A0DA-96697AC43DA1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B3C88A-23DB-4710-810D-18E1FA081FF2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" xr2:uid="{5B4E5AD1-9CC3-496A-B7F0-65442161F04A}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>Component Pin</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>PA1_FAULT</t>
+  </si>
+  <si>
+    <t>Motor Control (Mike will have to fill this in)</t>
   </si>
 </sst>
 </file>
@@ -570,11 +573,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CD125D1-636B-4535-A95A-3A65B99A69ED}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K16" sqref="K16"/>
+      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,7 +901,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -915,9 +918,75 @@
         <v>24</v>
       </c>
     </row>
+    <row r="23" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>31</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>21</v>
+      </c>
+      <c r="D25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>28</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>15</v>
+      </c>
+      <c r="D27">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>13</v>
+      </c>
+      <c r="D28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>11</v>
+      </c>
+      <c r="D29">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>12</v>
+      </c>
+      <c r="D30">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A23:E23"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A12:E12"/>

</xml_diff>